<commit_message>
reordering of trial-types in stimuli file
</commit_message>
<xml_diff>
--- a/stimuli.xlsx
+++ b/stimuli.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -229,8 +229,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -423,7 +425,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -509,6 +511,7 @@
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -594,6 +597,7 @@
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -926,7 +930,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1497,7 +1501,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="4">
         <v>2</v>
@@ -1532,7 +1536,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B18" s="4">
         <v>2</v>
@@ -1567,7 +1571,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4">
         <v>2</v>
@@ -1602,7 +1606,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4">
         <v>2</v>
@@ -1637,7 +1641,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4">
         <v>2</v>
@@ -1672,7 +1676,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="4">
         <v>3</v>
@@ -1681,33 +1685,33 @@
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>
@@ -1716,33 +1720,33 @@
         <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B24" s="4">
         <v>3</v>
@@ -1751,33 +1755,33 @@
         <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4">
         <v>3</v>
@@ -1786,33 +1790,33 @@
         <v>20</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="4">
         <v>3</v>
@@ -1821,33 +1825,33 @@
         <v>20</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B27" s="4">
         <v>4</v>
@@ -1856,33 +1860,33 @@
         <v>20</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B28" s="4">
         <v>4</v>
@@ -1891,33 +1895,33 @@
         <v>20</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B29" s="4">
         <v>4</v>
@@ -1926,33 +1930,33 @@
         <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B30" s="4">
         <v>4</v>
@@ -1961,33 +1965,33 @@
         <v>20</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B31" s="4">
         <v>4</v>
@@ -1996,28 +2000,28 @@
         <v>20</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.1 separated block_layout and exemplars
working. next step is to change multiplier so that it’s based on the
number of exemplars. Then block length will be fixed by code, but n of
exemplars can vary freely.
</commit_message>
<xml_diff>
--- a/stimuli.xlsx
+++ b/stimuli.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="6080" windowWidth="16560" windowHeight="4720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Correct</t>
   </si>
@@ -66,9 +66,6 @@
     <t>I am not a failure</t>
   </si>
   <si>
-    <t>stimulus</t>
-  </si>
-  <si>
     <t>I am interesting</t>
   </si>
   <si>
@@ -114,26 +111,29 @@
     <t>I am good</t>
   </si>
   <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>false_label</t>
-  </si>
-  <si>
-    <t>trial_type</t>
-  </si>
-  <si>
-    <t>true_label</t>
+    <t>trial_type_1_exemplars</t>
+  </si>
+  <si>
+    <t>trial_type_2_exemplars</t>
+  </si>
+  <si>
+    <t>trial_type_3_exemplars</t>
+  </si>
+  <si>
+    <t>trial_type_4_exemplars</t>
+  </si>
+  <si>
+    <t>trial_type_5_exemplars</t>
+  </si>
+  <si>
+    <t>trial_type_6_exemplars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,59 +159,16 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1890A8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6666"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6666FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8000FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0080FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,7 +180,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="207">
+  <cellStyleXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -431,46 +388,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="207">
+  <cellStyles count="221">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -574,6 +514,13 @@
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -677,6 +624,13 @@
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1006,451 +960,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="1" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
-        <v>1</v>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="11">
-        <v>2</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="11">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="11">
-        <v>2</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="11">
-        <v>2</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="11">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="15">
-        <v>3</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="15">
-        <v>3</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="15">
-        <v>3</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="15">
-        <v>3</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="17" t="s">
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="15">
-        <v>3</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="19">
-        <v>4</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="19">
-        <v>4</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="19">
-        <v>4</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="19">
-        <v>4</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="19">
-        <v>4</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="22">
-        <v>5</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="22">
-        <v>5</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="22">
-        <v>5</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="22">
-        <v>5</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="21" t="s">
+      <c r="F6" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B26" s="22">
-        <v>5</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="7">
-        <v>6</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="7">
-        <v>6</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="7">
-        <v>6</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="7">
-        <v>6</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="7">
-        <v>6</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>